<commit_message>
Added cost model and provenance sections to SBOM
</commit_message>
<xml_diff>
--- a/docs/3_ethics_and_licensing/software_and_data_inventory/SBOM.xlsx
+++ b/docs/3_ethics_and_licensing/software_and_data_inventory/SBOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\eaca\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\eaca\com2020\docs\3_ethics_and_licensing\software_and_data_inventory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{06BF51F8-8A7C-4EAB-BF9A-55244EACC905}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1255DB20-A82C-4829-A58C-E4F4A07EEBF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="15400" windowHeight="15370" xr2:uid="{4AABBBD3-43E7-4B06-BF25-05781DA341C4}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{4AABBBD3-43E7-4B06-BF25-05781DA341C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="69">
   <si>
     <t>Software Bill of Materials</t>
   </si>
@@ -173,9 +173,6 @@
     <t>9.0.2</t>
   </si>
   <si>
-    <t>Licence type</t>
-  </si>
-  <si>
     <t>Apache 2.0</t>
   </si>
   <si>
@@ -219,6 +216,33 @@
   </si>
   <si>
     <t>Google</t>
+  </si>
+  <si>
+    <t>Cost model</t>
+  </si>
+  <si>
+    <t>Provenance</t>
+  </si>
+  <si>
+    <t>Free to use and distribute, as per licence</t>
+  </si>
+  <si>
+    <t>Free to use, but not distribute, as per licence - this is a testing framework and as such will not be distributed.</t>
+  </si>
+  <si>
+    <t>Official licence link</t>
+  </si>
+  <si>
+    <t>Free up to 10k grants per day</t>
+  </si>
+  <si>
+    <t>FasterXML LLC https://github.com/FasterXML/</t>
+  </si>
+  <si>
+    <t>junit.org</t>
+  </si>
+  <si>
+    <t>The Apache Software Foundation https://www.apache.org/licenses/</t>
   </si>
 </sst>
 </file>
@@ -409,71 +433,90 @@
     </border>
     <border>
       <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -808,10 +851,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04A40349-3CAD-48C4-ACC5-4B7769909782}">
-  <dimension ref="B1:L38"/>
+  <dimension ref="B1:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -820,394 +863,454 @@
     <col min="2" max="2" width="12.1796875" customWidth="1"/>
     <col min="3" max="3" width="21.81640625" customWidth="1"/>
     <col min="4" max="4" width="28.54296875" customWidth="1"/>
-    <col min="5" max="5" width="7.81640625" customWidth="1"/>
+    <col min="5" max="5" width="10.6328125" customWidth="1"/>
     <col min="6" max="6" width="12.7265625" customWidth="1"/>
-    <col min="7" max="7" width="61.1796875" customWidth="1"/>
+    <col min="7" max="7" width="35" customWidth="1"/>
+    <col min="8" max="8" width="44.36328125" customWidth="1"/>
+    <col min="9" max="9" width="32.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:12" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="9" t="s">
+    <row r="1" spans="2:9" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="11"/>
-    </row>
-    <row r="3" spans="2:12" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C2" s="11"/>
+      <c r="D2" s="17"/>
+    </row>
+    <row r="3" spans="2:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="3"/>
-    </row>
-    <row r="4" spans="2:12" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="4" t="s">
+      <c r="D3" s="16"/>
+    </row>
+    <row r="4" spans="2:9" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="6"/>
-    </row>
-    <row r="5" spans="2:12" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="6" spans="2:12" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="14" t="s">
+      <c r="D4" s="16"/>
+    </row>
+    <row r="5" spans="2:9" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="6" spans="2:9" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-    </row>
-    <row r="7" spans="2:12" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="12" t="s">
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="8"/>
+    </row>
+    <row r="7" spans="2:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F7" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="G7" s="17" t="s">
+      <c r="F7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-    </row>
-    <row r="8" spans="2:12" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G7" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H7" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="I7" s="28" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="16" t="s">
         <v>23</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="G8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-    </row>
-    <row r="9" spans="2:12" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H8" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="I8" s="19" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="16" t="s">
         <v>23</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="G9" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-    </row>
-    <row r="10" spans="2:12" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H9" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="I9" s="19" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="16" t="s">
         <v>24</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="G10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-    </row>
-    <row r="11" spans="2:12" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H10" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="16" t="s">
         <v>25</v>
       </c>
       <c r="F11" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="G11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G11" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-    </row>
-    <row r="12" spans="2:12" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H11" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="I11" s="19" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="16" t="s">
         <v>26</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="G12" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G12" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-    </row>
-    <row r="13" spans="2:12" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="4" t="s">
+      <c r="H12" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="I12" s="19" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F13" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="G13" s="6" t="s">
+      <c r="F13" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-    </row>
-    <row r="14" spans="2:12" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="15" spans="2:12" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="25" t="s">
+      <c r="H13" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="I13" s="21" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
+    </row>
+    <row r="15" spans="2:9" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B15" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="21"/>
-    </row>
-    <row r="16" spans="2:12" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="7" t="s">
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="8"/>
+    </row>
+    <row r="16" spans="2:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8" t="s">
+      <c r="D16" s="31"/>
+      <c r="E16" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="F16" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="G16" s="24" t="s">
+      <c r="F16" s="30" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G16" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="H16" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="I16" s="28" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2" t="s">
+      <c r="D17" s="32"/>
+      <c r="E17" s="16" t="s">
         <v>33</v>
       </c>
       <c r="F17" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+        <v>47</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="H17" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2" t="s">
+      <c r="D18" s="33"/>
+      <c r="E18" s="16" t="s">
         <v>36</v>
       </c>
       <c r="F18" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+      <c r="G18" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="H18" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2" t="s">
+      <c r="D19" s="33"/>
+      <c r="E19" s="16" t="s">
         <v>37</v>
       </c>
       <c r="F19" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+      <c r="G19" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="H19" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2" t="s">
+      <c r="D20" s="33"/>
+      <c r="E20" s="16" t="s">
         <v>39</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+      <c r="G20" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="H20" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2" t="s">
+      <c r="D21" s="33"/>
+      <c r="E21" s="16" t="s">
         <v>43</v>
       </c>
       <c r="F21" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B22" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G21" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="H21" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B22" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5" t="s">
+      <c r="D22" s="34"/>
+      <c r="E22" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="F22" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G22" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="24" spans="2:7" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B24" s="27" t="s">
+      <c r="G22" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H22" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" ht="26.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="24" spans="2:9" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B24" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" s="15"/>
+      <c r="D24" s="22"/>
+    </row>
+    <row r="25" spans="2:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="C24" s="28"/>
-    </row>
-    <row r="25" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="1" t="s">
+      <c r="C25" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="D25" s="35" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B26" s="3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="26" spans="2:7" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B26" s="29" t="s">
+      <c r="C26" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C26" s="30" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="28" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="29" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="30" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="31" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="32" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.35"/>
+      <c r="D26" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" ht="20" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="28" spans="2:9" ht="20" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="29" spans="2:9" ht="20" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="30" spans="2:9" ht="20" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="31" spans="2:9" ht="20" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="32" spans="2:9" ht="20" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="33" ht="20" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="34" ht="20" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="35" ht="20" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1215,11 +1318,18 @@
     <row r="37" ht="20" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="38" ht="20" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="B24:C24"/>
+  <mergeCells count="11">
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C22:D22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>